<commit_message>
Local Multiplayer and Camera Management
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>AI(optional)</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -134,6 +137,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:E17"/>
+  <dimension ref="C4:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,12 +435,6 @@
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D2">
-        <f>SUM(D5:D36)</f>
-        <v>17</v>
-      </c>
-    </row>
     <row r="4" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -464,7 +464,9 @@
       <c r="D6" s="1">
         <v>2</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
@@ -473,7 +475,9 @@
       <c r="D7" s="1">
         <v>0.5</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
@@ -564,6 +568,19 @@
         <v>2</v>
       </c>
       <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2">
+        <f>SUM(D5:D17)</f>
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <f>SUM(E5:E17)</f>
+        <v>3.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bomb Placement and Collison Check
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Task</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Bomb &amp; Brick FX(Optional)</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:E18"/>
+  <dimension ref="C4:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +500,9 @@
       <c r="D9" s="1">
         <v>1.5</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
@@ -506,7 +511,9 @@
       <c r="D10" s="1">
         <v>1.5</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
@@ -515,7 +522,9 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="12" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
@@ -571,17 +580,26 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+    <row r="18" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="2">
-        <f>SUM(D5:D17)</f>
-        <v>17</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="D19" s="2">
+        <f>SUM(D5:D18)</f>
+        <v>19</v>
+      </c>
+      <c r="E19" s="2">
         <f>SUM(E5:E17)</f>
-        <v>5.3</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI, HUD and Savedata
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -72,16 +72,22 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Bomb &amp; Brick FX(Optional)</t>
-  </si>
-  <si>
-    <t>Sounds(optional)</t>
-  </si>
-  <si>
-    <t>Future Tasks</t>
-  </si>
-  <si>
-    <t>Legends</t>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>AI which works as Player</t>
+  </si>
+  <si>
+    <t>Neutral characters</t>
+  </si>
+  <si>
+    <t>Sounds</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Future Task</t>
   </si>
 </sst>
 </file>
@@ -146,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,11 +169,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:I20"/>
+  <dimension ref="C4:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +464,8 @@
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:9" ht="18.75" x14ac:dyDescent="0.25">
@@ -472,6 +478,9 @@
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
@@ -483,6 +492,7 @@
       <c r="E5" s="1">
         <v>0.5</v>
       </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
@@ -494,6 +504,7 @@
       <c r="E6" s="1">
         <v>2.5</v>
       </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
@@ -505,8 +516,9 @@
       <c r="E7" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="3:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -515,6 +527,10 @@
       </c>
       <c r="E8" s="1">
         <v>2</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="I8" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
@@ -527,6 +543,10 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
+      <c r="F9" s="6"/>
+      <c r="I9" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
@@ -538,10 +558,10 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="I10" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
@@ -553,12 +573,12 @@
       <c r="E11" s="1">
         <v>0.5</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F11" s="6"/>
+      <c r="I11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
@@ -567,6 +587,10 @@
       </c>
       <c r="E12" s="1">
         <v>1.5</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="I12" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
@@ -579,6 +603,7 @@
       <c r="E13" s="1">
         <v>0.5</v>
       </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
@@ -587,7 +612,10 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
@@ -596,7 +624,10 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
@@ -605,9 +636,12 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
@@ -615,42 +649,23 @@
         <v>2</v>
       </c>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="3:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2">
+        <f>SUM(D5:D17)</f>
         <v>17</v>
       </c>
-      <c r="D18" s="1">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="3:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="2">
-        <f>SUM(D5:D19)</f>
-        <v>20</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="E18" s="2">
         <f>SUM(E5:E17)</f>
-        <v>10.8</v>
-      </c>
+        <v>13.8</v>
+      </c>
+      <c r="F18" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H10:I10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Sounds and Pickups Chance reduced to 30%
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -453,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:I18"/>
+  <dimension ref="C4:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:F17"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
       </c>
       <c r="F11" s="6"/>
       <c r="I11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -589,9 +589,6 @@
         <v>1.5</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="I12" s="3" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
@@ -642,28 +639,38 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="3:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="1"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="3:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="2">
-        <f>SUM(D5:D17)</f>
+      <c r="D19" s="2">
+        <f>SUM(D5:D18)</f>
         <v>17</v>
       </c>
-      <c r="E18" s="2">
-        <f>SUM(E5:E17)</f>
-        <v>13.8</v>
-      </c>
-      <c r="F18" s="6"/>
+      <c r="E19" s="2">
+        <f>SUM(E5:E18)</f>
+        <v>14.3</v>
+      </c>
+      <c r="F19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pickups destroyed if in bomb range
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -66,9 +66,6 @@
     <t>Save Data</t>
   </si>
   <si>
-    <t>AI(optional)</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Future Task</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -111,18 +111,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -152,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,9 +158,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -455,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,8 +469,8 @@
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>17</v>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="30" x14ac:dyDescent="0.25">
@@ -492,7 +483,7 @@
       <c r="E5" s="1">
         <v>0.5</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
@@ -504,7 +495,7 @@
       <c r="E6" s="1">
         <v>2.5</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
@@ -516,7 +507,7 @@
       <c r="E7" s="1">
         <v>0.3</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="3:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
@@ -528,9 +519,9 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="I8" s="7" t="s">
-        <v>22</v>
+      <c r="F8" s="5"/>
+      <c r="I8" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
@@ -543,9 +534,9 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="5"/>
       <c r="I9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
@@ -558,9 +549,9 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="I10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
@@ -573,9 +564,9 @@
       <c r="E11" s="1">
         <v>0.5</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="5"/>
       <c r="I11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -588,7 +579,7 @@
       <c r="E12" s="1">
         <v>1.5</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
@@ -600,7 +591,7 @@
       <c r="E13" s="1">
         <v>0.5</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
@@ -612,7 +603,7 @@
       <c r="E14" s="1">
         <v>0.5</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
@@ -624,7 +615,7 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
@@ -636,41 +627,41 @@
       <c r="E16" s="1">
         <v>1.5</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
         <v>0.5</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="6"/>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="3:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2">
         <f>SUM(D5:D18)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E19" s="2">
         <f>SUM(E5:E18)</f>
-        <v>14.3</v>
-      </c>
-      <c r="F19" s="6"/>
+        <v>14.8</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>